<commit_message>
daily changes "var and datatypes" dec_31
</commit_message>
<xml_diff>
--- a/Concepts_LP.xlsx
+++ b/Concepts_LP.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Python</t>
   </si>
   <si>
-    <t>Data Types</t>
-  </si>
-  <si>
     <t>Control Structures</t>
   </si>
   <si>
@@ -62,6 +59,12 @@
   </si>
   <si>
     <t>datatypes.py</t>
+  </si>
+  <si>
+    <t>Variables and data types</t>
+  </si>
+  <si>
+    <t>controlstructures.py</t>
   </si>
 </sst>
 </file>
@@ -439,13 +442,13 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
@@ -456,24 +459,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4">
         <v>45649</v>
@@ -487,54 +490,56 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4">
         <v>45652</v>
       </c>
       <c r="D3" s="4">
-        <v>45652</v>
+        <v>45656</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C4" s="4">
-        <v>45654</v>
+        <v>45657</v>
       </c>
       <c r="D4" s="4">
-        <v>45656</v>
+        <v>45657</v>
       </c>
       <c r="E4" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="4">
-        <v>45657</v>
+        <v>45658</v>
       </c>
       <c r="D5" s="4">
         <v>45658</v>
       </c>
       <c r="E5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="4">
@@ -549,7 +554,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="4">
@@ -564,7 +569,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="4">
@@ -579,7 +584,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="4">
@@ -594,7 +599,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="4">

</xml_diff>

<commit_message>
daily changes jan_1 control structures
</commit_message>
<xml_diff>
--- a/Concepts_LP.xlsx
+++ b/Concepts_LP.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Python</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Control Structures</t>
   </si>
@@ -31,21 +28,12 @@
     <t>OOPS</t>
   </si>
   <si>
-    <t>Exception handling</t>
-  </si>
-  <si>
-    <t>File handling</t>
-  </si>
-  <si>
     <t>file name</t>
   </si>
   <si>
     <t>Collection Module</t>
   </si>
   <si>
-    <t>Decorator/Generator</t>
-  </si>
-  <si>
     <t>collections.py</t>
   </si>
   <si>
@@ -65,6 +53,33 @@
   </si>
   <si>
     <t>controlstructures.py</t>
+  </si>
+  <si>
+    <t>File and Exception handling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Class_and_methods </t>
+  </si>
+  <si>
+    <t>functions.py</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>namedtuple , default dict , counter , dequeu, chained map etc…</t>
+  </si>
+  <si>
+    <t>string , int , float , dict, tuple , set , list, array…</t>
+  </si>
+  <si>
+    <t>if , else , elif , try, except , with, pass , break , continue…</t>
+  </si>
+  <si>
+    <t>map , lambda , filter, decorator , generator, *args, **kwargs…</t>
+  </si>
+  <si>
+    <t>Python-Concepts</t>
   </si>
 </sst>
 </file>
@@ -439,44 +454,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4">
         <v>45649</v>
@@ -487,13 +506,16 @@
       <c r="E2" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C3" s="4">
         <v>45652</v>
@@ -504,13 +526,16 @@
       <c r="E3" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" s="4">
         <v>45657</v>
@@ -521,12 +546,17 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="C5" s="4">
         <v>45658</v>
       </c>
@@ -536,8 +566,11 @@
       <c r="E5" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -546,71 +579,60 @@
         <v>45659</v>
       </c>
       <c r="D6" s="4">
-        <v>45661</v>
+        <v>45660</v>
       </c>
       <c r="E6" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="4">
+        <v>45661</v>
+      </c>
+      <c r="D7" s="4">
         <v>45662</v>
       </c>
-      <c r="D7" s="4">
-        <v>45665</v>
-      </c>
       <c r="E7" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="4">
-        <v>45666</v>
+        <v>45663</v>
       </c>
       <c r="D8" s="4">
-        <v>45666</v>
+        <v>45664</v>
       </c>
       <c r="E8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="4">
-        <v>45667</v>
+        <v>45665</v>
       </c>
       <c r="D9" s="4">
-        <v>45667</v>
+        <v>45666</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4">
-        <v>45668</v>
-      </c>
-      <c r="D10" s="4">
-        <v>45669</v>
-      </c>
-      <c r="E10" s="2">
         <v>2</v>
       </c>
+      <c r="F9" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A2:E11">

</xml_diff>